<commit_message>
milestone 5, added changes detailed in doc.
</commit_message>
<xml_diff>
--- a/documentation/Sound-Asset-List.xlsx
+++ b/documentation/Sound-Asset-List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="41">
   <si>
     <t>Sound Name</t>
   </si>
@@ -59,12 +59,6 @@
     <t>whoosh noise, similar frequency throughout sound but increases a bit, alerts user they are hovering an option</t>
   </si>
   <si>
-    <t>crashing waves on the beach, relaxing mood, will be used as background ambience for interface and even game(maybe)</t>
-  </si>
-  <si>
-    <t>whenever player assets move, they will be making a seamless sand moving sound, sound of crab walking on beach(not realistic)</t>
-  </si>
-  <si>
     <t>bright sounding artificial excitement noise, sound is played when crab enters ungated hole and progresses to next level</t>
   </si>
   <si>
@@ -92,9 +86,6 @@
     <t>beach-waves</t>
   </si>
   <si>
-    <t>gravel-walk(footsteps1,2,3)</t>
-  </si>
-  <si>
     <t>button-activated</t>
   </si>
   <si>
@@ -135,6 +126,27 @@
   </si>
   <si>
     <t>in Unity but incomplete</t>
+  </si>
+  <si>
+    <t>wall collision</t>
+  </si>
+  <si>
+    <t>small bump noise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">crashing waves on the beach, relaxing mood, will be used as background ambience </t>
+  </si>
+  <si>
+    <t>gravel-walk-param2(footsteps1,2,3)</t>
+  </si>
+  <si>
+    <t>gravel-walk-param(footsteps1,2,3)</t>
+  </si>
+  <si>
+    <t>whenever player assets move, they will be making a seamless sand moving sound, sound of crab walking on beach(not realistic), meant for crab x</t>
+  </si>
+  <si>
+    <t>whenever player assets move, they will be making a seamless sand moving sound, sound of crab walking on beach(not realistic), meant for crab y</t>
   </si>
 </sst>
 </file>
@@ -492,8 +504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -514,16 +526,16 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -534,7 +546,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
@@ -543,7 +555,7 @@
         <v>3</v>
       </c>
       <c r="F3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -551,7 +563,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
@@ -560,7 +572,7 @@
         <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -568,16 +580,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="D5" t="s">
         <v>5</v>
       </c>
       <c r="F5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -585,16 +597,16 @@
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>6</v>
       </c>
       <c r="F6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -602,16 +614,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="D7" t="s">
         <v>4</v>
       </c>
       <c r="F7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -619,16 +631,16 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="D8" t="s">
         <v>4</v>
       </c>
       <c r="F8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -636,16 +648,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D9" t="s">
         <v>4</v>
       </c>
       <c r="F9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -653,16 +665,16 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="D10" t="s">
         <v>4</v>
       </c>
       <c r="F10" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -670,16 +682,16 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D11" t="s">
         <v>4</v>
       </c>
       <c r="F11" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -687,16 +699,16 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
         <v>26</v>
       </c>
-      <c r="C12" t="s">
-        <v>13</v>
-      </c>
       <c r="D12" t="s">
         <v>4</v>
       </c>
       <c r="F12" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -704,23 +716,45 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" t="s">
         <v>35</v>
       </c>
-      <c r="D13" t="s">
-        <v>4</v>
-      </c>
-      <c r="F13" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
+      <c r="D15" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
@@ -737,7 +771,7 @@
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding final fixes based off milestone 5 feedback
</commit_message>
<xml_diff>
--- a/documentation/Sound-Asset-List.xlsx
+++ b/documentation/Sound-Asset-List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="40">
   <si>
     <t>Sound Name</t>
   </si>
@@ -125,15 +125,9 @@
     <t>pitched down click sound will be played when button is unpressed</t>
   </si>
   <si>
-    <t>in Unity but incomplete</t>
-  </si>
-  <si>
     <t>wall collision</t>
   </si>
   <si>
-    <t>small bump noise</t>
-  </si>
-  <si>
     <t xml:space="preserve">crashing waves on the beach, relaxing mood, will be used as background ambience </t>
   </si>
   <si>
@@ -147,6 +141,9 @@
   </si>
   <si>
     <t>whenever player assets move, they will be making a seamless sand moving sound, sound of crab walking on beach(not realistic), meant for crab y</t>
+  </si>
+  <si>
+    <t>small bump noise with rock</t>
   </si>
 </sst>
 </file>
@@ -505,7 +502,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,7 +580,7 @@
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D5" t="s">
         <v>5</v>
@@ -614,10 +611,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D7" t="s">
         <v>4</v>
@@ -631,10 +628,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D8" t="s">
         <v>4</v>
@@ -674,7 +671,7 @@
         <v>4</v>
       </c>
       <c r="F10" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -691,7 +688,7 @@
         <v>4</v>
       </c>
       <c r="F11" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -747,10 +744,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C15" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D15" t="s">
         <v>4</v>

</xml_diff>